<commit_message>
quiz initial presenter work
</commit_message>
<xml_diff>
--- a/quiz_entries.xlsx
+++ b/quiz_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\matlab\matlab_quiz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/Documents/repos/matlab/matlab_quiz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92183B60-D6D2-4912-AD54-AE217529AE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291F909B-7A13-C947-B3B7-78382685B41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35940" yWindow="2390" windowWidth="28800" windowHeight="15460" xr2:uid="{227AB921-754E-4DEE-B4BC-2BC1A0EFF452}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{227AB921-754E-4DEE-B4BC-2BC1A0EFF452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>question</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>function</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>jah</t>
+  </si>
+  <si>
+    <t>creation_date</t>
   </si>
 </sst>
 </file>
@@ -140,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -148,6 +157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,22 +472,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F2FA4D-A0A0-4838-A3D3-D2DDFEDFE174}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="106.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="94.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="106.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="94.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,8 +504,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -507,8 +524,14 @@
       <c r="E2" s="1">
         <v>2</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3">
+        <v>44631</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -524,8 +547,14 @@
       <c r="E3" s="1">
         <v>3</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3">
+        <v>44631</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -537,6 +566,12 @@
       </c>
       <c r="E4" s="1">
         <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3">
+        <v>44631</v>
       </c>
     </row>
   </sheetData>
@@ -552,13 +587,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -569,7 +604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>2</v>
       </c>
@@ -577,7 +612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>3</v>
       </c>

</xml_diff>